<commit_message>
update on kill switch, notification, app crushing report...
</commit_message>
<xml_diff>
--- a/features/backlog/android/about_us.xlsx
+++ b/features/backlog/android/about_us.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472AD0C-66BB-43AB-A846-42FC420606DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFEA747-BC9A-4A92-A969-773EFF00D16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1029,7 +1029,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add expected value in the file...
</commit_message>
<xml_diff>
--- a/features/backlog/android/about_us.xlsx
+++ b/features/backlog/android/about_us.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFEA747-BC9A-4A92-A969-773EFF00D16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B82541D-9CFC-48C0-8DDC-491DE00EE56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>check the about us menu is avaiable or not for free user or not.</t>
   </si>
   <si>
-    <t>check the about us menu is avaiable or not for primium user or not.</t>
-  </si>
-  <si>
     <t>1. Open the app
 2. login to the app with valid credentials
 3. find the menu for about us</t>
@@ -81,25 +78,13 @@
     <t>placeholder text should be shown properly</t>
   </si>
   <si>
-    <t>Check the design of the subscriptuon code field is as executed or not</t>
-  </si>
-  <si>
     <t>check the subscriptuon field in the about us page design should be as per the  specification</t>
-  </si>
-  <si>
-    <t>Check if the subscriptuon field in the about us page field is mandatory. Then red ” * ” should be displayed.</t>
-  </si>
-  <si>
-    <t>Check whether placeholder text should be shown properly or not for the subscription field in the about us page in the about us page</t>
   </si>
   <si>
     <t>check the width of the subscriptuon field in the about us page</t>
   </si>
   <si>
     <t>check the height of the subscriptuon field in the about us page</t>
-  </si>
-  <si>
-    <t>Test case scenario: About US Screenn Android</t>
   </si>
   <si>
     <t>1. Open the app
@@ -130,6 +115,30 @@
   </si>
   <si>
     <t>SYMMOBABT-009</t>
+  </si>
+  <si>
+    <t>Test case scenario: About Us Screen Android</t>
+  </si>
+  <si>
+    <t>check the about us menu is avaiable or not for premium user or not.</t>
+  </si>
+  <si>
+    <t>should the about us menu is avaiable for free users</t>
+  </si>
+  <si>
+    <t>check the about us menu is avaiable or not for expired user or not.</t>
+  </si>
+  <si>
+    <t>should the about us menu is avaiable for expired users</t>
+  </si>
+  <si>
+    <t>check if the subscriptuon field in the about us page field is mandatory. Then red ” * ” should be displayed.</t>
+  </si>
+  <si>
+    <t>check whether placeholder text should be shown properly or not for the subscription field in the about us page in the about us page</t>
+  </si>
+  <si>
+    <t>check the design of the subscriptuon code field is as executed or not</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1037,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G2"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1055,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1144,7 +1153,7 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1155,10 +1164,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>8</v>
@@ -1186,21 +1195,21 @@
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
@@ -1228,19 +1237,19 @@
     </row>
     <row r="6" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>8</v>
@@ -1268,19 +1277,19 @@
     </row>
     <row r="7" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>8</v>
@@ -1308,19 +1317,19 @@
     </row>
     <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>8</v>
@@ -1348,19 +1357,19 @@
     </row>
     <row r="9" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>8</v>
@@ -1388,19 +1397,19 @@
     </row>
     <row r="10" spans="1:26" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>8</v>
@@ -1428,19 +1437,19 @@
     </row>
     <row r="11" spans="1:26" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>8</v>
@@ -1468,19 +1477,19 @@
     </row>
     <row r="12" spans="1:26" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>8</v>
@@ -1508,19 +1517,19 @@
     </row>
     <row r="13" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>8</v>

</xml_diff>